<commit_message>
Added comments and continued design (USB-UART converter)
</commit_message>
<xml_diff>
--- a/board/stm-universal-can-board/Partlist.xlsx
+++ b/board/stm-universal-can-board/Partlist.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03BFE01-3528-47F0-B847-08D59913C997}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A44007-AB63-49B7-9174-4D74889442E9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -115,7 +115,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,6 +145,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -167,16 +191,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -461,17 +489,17 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A7" sqref="A7:G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="3" width="47.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" customWidth="1"/>
+    <col min="3" max="3" width="47.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,7 +522,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -512,7 +540,7 @@
       </c>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -530,7 +558,7 @@
       </c>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -548,7 +576,7 @@
       </c>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -566,7 +594,7 @@
       </c>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -589,25 +617,26 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="8">
         <v>0.14099999999999999</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F7" s="10"/>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -625,127 +654,127 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D9" s="2"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D10" s="2"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D11" s="2"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D12" s="2"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D13" s="2"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D14" s="2"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D15" s="2"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D16" s="2"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D17" s="2"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D18" s="2"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D19" s="2"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D20" s="2"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D21" s="2"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D22" s="2"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D23" s="2"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D24" s="2"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D25" s="2"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D26" s="2"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D27" s="2"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D28" s="2"/>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D29" s="2"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D30" s="2"/>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D31" s="2"/>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D32" s="2"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D33" s="2"/>
       <c r="F33" s="5"/>
     </row>
-    <row r="34" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D34" s="2"/>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D35" s="2"/>
       <c r="F35" s="5"/>
     </row>
-    <row r="36" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D36" s="2"/>
       <c r="F36" s="5"/>
     </row>
-    <row r="37" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D37" s="2"/>
       <c r="F37" s="5"/>
     </row>
-    <row r="38" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D38" s="2"/>
       <c r="F38" s="5"/>
     </row>
-    <row r="39" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D39" s="2"/>
       <c r="F39" s="5"/>
     </row>

</xml_diff>